<commit_message>
Videogames NNSnake and CNN
</commit_message>
<xml_diff>
--- a/Temp_folder/Caso Tinder.xlsx
+++ b/Temp_folder/Caso Tinder.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dave_PersonalCarpet\code\2020_01\Temp_folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dave\code\2020_01\Temp_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EFE" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t xml:space="preserve">Oportunidades </t>
   </si>
@@ -118,39 +118,10 @@
     <t>Uso de tecnologías robóticas con asociados de Alemania y Francia.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">La experiencia del mercado Mexicano y su elevado </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>expertise</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> elevan los estándares del producto</t>
-    </r>
-  </si>
-  <si>
     <t>Cambios en el manejo de la gestión sumamente rápidos. Políticas enfocadas a la no burocratización pero si a la rapidez de las acciones.</t>
   </si>
   <si>
     <t>Compromiso e involucramiento del personal reflejados en su filosofía de trabajo.</t>
-  </si>
-  <si>
-    <t>Se sacrifican ciertos atributos de atributos que ofrecen los productos de los todistas.</t>
   </si>
   <si>
     <t>(P) Durante un tiempo se intento esparcir mala fama a la empresa por la epidemia del Cólera.</t>
@@ -346,16 +317,37 @@
     <t>Alumno: José David Mamani Vilca</t>
   </si>
   <si>
-    <t>Ambos fundadores se conocieron desde hace varios años.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilizar la amplia variedad de tecnologías en los aparatos móviles para facilitar las relaciones humanas </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Tecnologías </t>
+    <t>Nuevas tecnologías prestas en los aparatos móviles para facilitar el proceso de las relaciones humanas.</t>
+  </si>
+  <si>
+    <t>El concepto de la aplicación era completamente novedoso para su época (2012).</t>
+  </si>
+  <si>
+    <t>Dos de sus fundadores eran compañeros y estaban envueltos en el mundo del emprendimiento tecnológico.</t>
+  </si>
+  <si>
+    <t>Estrategia enfocada en utilizar a los universitarios como herramientas de marketing.</t>
+  </si>
+  <si>
+    <t>Gamificación para que la aplicación resulta más atractiva hacia sus usuarios.</t>
+  </si>
+  <si>
+    <t>Cambiar dicha concepción al masificar su uso en la generación milenial</t>
+  </si>
+  <si>
+    <t>Estigma social, en donde los usuarios con vistos como individuos de pobres habilidades sociales.</t>
+  </si>
+  <si>
+    <t>*Encajar de forma perfecta en su público objetivo.</t>
+  </si>
+  <si>
+    <t>Caso Tinder</t>
+  </si>
+  <si>
+    <t>Marketing de guerrillas al promocionar eventos con potencial de nuevos usuarios.</t>
   </si>
 </sst>
 </file>
@@ -395,7 +387,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -625,22 +617,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -692,9 +687,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -978,138 +987,143 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="140.28515625" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>82</v>
+      <c r="B1" s="22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="4"/>
+      <c r="A2" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="32"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="30" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="32"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="B6" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="B7" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="35" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="27"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="29"/>
+      <c r="B10" s="27"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="29"/>
+      <c r="B11" s="27"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="29"/>
+      <c r="B12" s="27"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="29"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>34</v>
+      <c r="B15" s="35" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="29" t="s">
-        <v>20</v>
-      </c>
+      <c r="B16" s="27"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>84</v>
+      <c r="B17" s="29"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1120,141 +1134,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="139.85546875" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="32"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="B8" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="B9" s="35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="B10" s="27"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="B11" s="27"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="B12" s="27"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="B13" s="27"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>32</v>
-      </c>
+      <c r="B14" s="29"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="25" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="29" t="s">
-        <v>33</v>
-      </c>
+      <c r="B16" s="27"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="29" t="s">
-        <v>26</v>
-      </c>
+      <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>27</v>
-      </c>
+      <c r="B18" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1276,339 +1275,339 @@
   <sheetData>
     <row r="2" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="5:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="10" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="5:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="H6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J6" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="5:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="16"/>
+      <c r="F13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="5:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="16"/>
+      <c r="F22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="19"/>
+      <c r="J22" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="E24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="5:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="5:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="5:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="5:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="18"/>
-      <c r="F13" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E14" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="5:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="5:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="18"/>
-      <c r="F22" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E23" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I23" s="10" t="s">
+      <c r="I25" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J25" s="2" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="5:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="E24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="5:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>